<commit_message>
fixed deterministic scenario QFT runs to use in tornado plots
</commit_message>
<xml_diff>
--- a/inst/extdata/scenario_input_values.xlsx
+++ b/inst/extdata/scenario_input_values.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n8tha\Documents\R\LTBIdiagTST\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\R\LTBIdiagTST\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F914B12-0E9B-4D72-88DB-6819FBD81F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E429BD9-78E2-4DD8-A4BF-A4C982131017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenario_input_values" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId1"/>
+    <sheet name="scenario_input_values" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>scenario</t>
   </si>
@@ -53,16 +54,7 @@
     <t>pComp_chemo</t>
   </si>
   <si>
-    <t>pLTBI</t>
-  </si>
-  <si>
     <t>Sp_cost</t>
-  </si>
-  <si>
-    <t>LTBIcomp_cost</t>
-  </si>
-  <si>
-    <t>LTBIincomp_cost</t>
   </si>
   <si>
     <t>pAccept_chemo</t>
@@ -74,13 +66,25 @@
     <t>Hep</t>
   </si>
   <si>
-    <t>TST</t>
+    <t>TB_cost</t>
   </si>
   <si>
-    <t>Ns_cost</t>
+    <t>LTBIcompl_cost</t>
   </si>
   <si>
-    <t>TB_cost</t>
+    <t>LTBIincompl_cost</t>
+  </si>
+  <si>
+    <t>For quantiferon only decision tree</t>
+  </si>
+  <si>
+    <t>PPV_QFT</t>
+  </si>
+  <si>
+    <t>NPV_QFT</t>
+  </si>
+  <si>
+    <t>QFT_pos</t>
   </si>
 </sst>
 </file>
@@ -567,12 +571,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -920,18 +923,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D403AE-70D9-415D-BC68-39EC0B6504C1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,14 +965,14 @@
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -976,35 +999,35 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
@@ -1023,31 +1046,31 @@
         <v>0.8</v>
       </c>
       <c r="G2">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H2">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I2">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J2">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K2">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L2">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M2">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N2">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O2">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P2">
         <v>4925.76</v>
@@ -1075,31 +1098,31 @@
         <v>0.8</v>
       </c>
       <c r="G3">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H3">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I3">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J3">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K3">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L3">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M3">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N3">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O3">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P3">
         <v>4925.76</v>
@@ -1127,31 +1150,31 @@
         <v>0.8</v>
       </c>
       <c r="G4">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H4">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I4">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J4">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K4">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L4">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M4">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N4">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O4">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P4">
         <v>4925.76</v>
@@ -1177,31 +1200,31 @@
         <v>0.8</v>
       </c>
       <c r="G5">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H5">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I5">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J5">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K5">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L5">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M5">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N5">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O5">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P5">
         <v>4925.76</v>
@@ -1227,31 +1250,31 @@
         <v>0.8</v>
       </c>
       <c r="G6">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H6">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I6">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J6">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K6">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L6">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M6">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N6">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O6">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P6">
         <v>4925.76</v>
@@ -1277,31 +1300,31 @@
         <v>0.5</v>
       </c>
       <c r="G7">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H7">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I7">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J7">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K7">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L7">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M7">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N7">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O7">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P7">
         <v>4925.76</v>
@@ -1327,31 +1350,31 @@
         <v>0.9</v>
       </c>
       <c r="G8">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H8">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I8">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J8">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K8">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L8">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M8">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N8">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O8">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P8">
         <v>4925.76</v>
@@ -1376,32 +1399,32 @@
       <c r="F9">
         <v>0.8</v>
       </c>
-      <c r="G9" s="2">
-        <v>0.1</v>
+      <c r="G9">
+        <v>241.23</v>
       </c>
       <c r="H9">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I9">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J9">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K9">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L9">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M9">
-        <v>18.62</v>
-      </c>
-      <c r="N9">
-        <v>732</v>
+        <v>732</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.8</v>
       </c>
       <c r="O9">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P9">
         <v>4925.76</v>
@@ -1426,32 +1449,32 @@
       <c r="F10">
         <v>0.8</v>
       </c>
-      <c r="G10" s="2">
-        <v>0.5</v>
+      <c r="G10">
+        <v>241.23</v>
       </c>
       <c r="H10">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I10">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J10">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K10">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L10">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M10">
-        <v>18.62</v>
-      </c>
-      <c r="N10">
-        <v>732</v>
+        <v>732</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1</v>
       </c>
       <c r="O10">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P10">
         <v>4925.76</v>
@@ -1476,32 +1499,32 @@
       <c r="F11">
         <v>0.8</v>
       </c>
-      <c r="G11">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="G11" s="2">
         <v>200</v>
       </c>
+      <c r="H11">
+        <v>169.68</v>
+      </c>
       <c r="I11">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J11">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K11">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L11">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M11">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N11">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O11">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P11">
         <v>4925.76</v>
@@ -1526,32 +1549,32 @@
       <c r="F12">
         <v>0.8</v>
       </c>
-      <c r="G12">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="G12" s="2">
         <v>300</v>
       </c>
+      <c r="H12">
+        <v>169.68</v>
+      </c>
       <c r="I12">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J12">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K12">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L12">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M12">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N12">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O12">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P12">
         <v>4925.76</v>
@@ -1577,31 +1600,31 @@
         <v>0.8</v>
       </c>
       <c r="G13">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="H13">
-        <v>241.23</v>
-      </c>
-      <c r="I13" s="2">
+        <v>241.23</v>
+      </c>
+      <c r="H13" s="2">
         <v>100</v>
       </c>
+      <c r="I13">
+        <v>84.84</v>
+      </c>
       <c r="J13">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K13">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L13">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M13">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N13">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O13">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P13">
         <v>4925.76</v>
@@ -1627,31 +1650,31 @@
         <v>0.8</v>
       </c>
       <c r="G14">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="H14">
-        <v>241.23</v>
-      </c>
-      <c r="I14" s="2">
+        <v>241.23</v>
+      </c>
+      <c r="H14" s="2">
         <v>200</v>
       </c>
+      <c r="I14">
+        <v>84.84</v>
+      </c>
       <c r="J14">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K14">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L14">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M14">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N14">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O14">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P14">
         <v>4925.76</v>
@@ -1677,31 +1700,31 @@
         <v>0.8</v>
       </c>
       <c r="G15">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H15">
-        <v>241.23</v>
-      </c>
-      <c r="I15">
-        <v>169.68</v>
-      </c>
-      <c r="J15" s="2">
+        <v>169.68</v>
+      </c>
+      <c r="I15" s="2">
         <v>50</v>
       </c>
+      <c r="J15">
+        <v>0.95</v>
+      </c>
       <c r="K15">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L15">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M15">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N15">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O15">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P15">
         <v>4925.76</v>
@@ -1727,31 +1750,31 @@
         <v>0.8</v>
       </c>
       <c r="G16">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H16">
-        <v>241.23</v>
-      </c>
-      <c r="I16">
-        <v>169.68</v>
-      </c>
-      <c r="J16" s="2">
+        <v>169.68</v>
+      </c>
+      <c r="I16" s="2">
         <v>150</v>
       </c>
+      <c r="J16">
+        <v>0.95</v>
+      </c>
       <c r="K16">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L16">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M16">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N16">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O16">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P16">
         <v>4925.76</v>
@@ -1777,31 +1800,31 @@
         <v>0.8</v>
       </c>
       <c r="G17">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H17">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I17">
-        <v>169.68</v>
-      </c>
-      <c r="J17">
-        <v>84.84</v>
-      </c>
-      <c r="K17" s="2">
+        <v>84.84</v>
+      </c>
+      <c r="J17" s="2">
         <v>0.5</v>
       </c>
+      <c r="K17">
+        <v>23.68</v>
+      </c>
       <c r="L17">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M17">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N17">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O17">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P17">
         <v>4925.76</v>
@@ -1827,31 +1850,31 @@
         <v>0.8</v>
       </c>
       <c r="G18">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H18">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I18">
-        <v>169.68</v>
-      </c>
-      <c r="J18">
-        <v>84.84</v>
-      </c>
-      <c r="K18" s="2">
+        <v>84.84</v>
+      </c>
+      <c r="J18" s="2">
         <v>1</v>
       </c>
+      <c r="K18">
+        <v>23.68</v>
+      </c>
       <c r="L18">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M18">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N18">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O18">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P18">
         <v>4925.76</v>
@@ -1877,31 +1900,31 @@
         <v>0.8</v>
       </c>
       <c r="G19">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H19">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I19">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J19">
-        <v>84.84</v>
-      </c>
-      <c r="K19">
-        <v>0.95</v>
-      </c>
-      <c r="L19" s="2">
-        <v>12</v>
+        <v>0.95</v>
+      </c>
+      <c r="K19" s="2">
+        <v>10</v>
+      </c>
+      <c r="L19">
+        <v>0.23</v>
       </c>
       <c r="M19">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N19">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O19">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P19">
         <v>4925.76</v>
@@ -1927,31 +1950,31 @@
         <v>0.8</v>
       </c>
       <c r="G20">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H20">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I20">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J20">
-        <v>84.84</v>
-      </c>
-      <c r="K20">
-        <v>0.95</v>
-      </c>
-      <c r="L20" s="2">
-        <v>45</v>
+        <v>0.95</v>
+      </c>
+      <c r="K20" s="2">
+        <v>100</v>
+      </c>
+      <c r="L20">
+        <v>0.23</v>
       </c>
       <c r="M20">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N20">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O20">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P20">
         <v>4925.76</v>
@@ -1977,31 +2000,31 @@
         <v>0.8</v>
       </c>
       <c r="G21">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H21">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I21">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J21">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K21">
-        <v>0.95</v>
-      </c>
-      <c r="L21">
-        <v>23.68</v>
-      </c>
-      <c r="M21" s="2">
-        <v>9</v>
+        <v>23.68</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M21">
+        <v>732</v>
       </c>
       <c r="N21">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O21">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P21">
         <v>4925.76</v>
@@ -2027,31 +2050,31 @@
         <v>0.8</v>
       </c>
       <c r="G22">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H22">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I22">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J22">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K22">
-        <v>0.95</v>
-      </c>
-      <c r="L22">
-        <v>23.68</v>
-      </c>
-      <c r="M22" s="2">
-        <v>37</v>
+        <v>23.68</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M22">
+        <v>732</v>
       </c>
       <c r="N22">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O22">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P22">
         <v>4925.76</v>
@@ -2077,31 +2100,31 @@
         <v>0.8</v>
       </c>
       <c r="G23">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H23">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I23">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J23">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K23">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L23">
-        <v>23.68</v>
-      </c>
-      <c r="M23">
-        <v>18.62</v>
-      </c>
-      <c r="N23" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="M23" s="2">
         <v>366</v>
       </c>
+      <c r="N23">
+        <v>0.9</v>
+      </c>
       <c r="O23">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P23">
         <v>4925.76</v>
@@ -2127,31 +2150,31 @@
         <v>0.8</v>
       </c>
       <c r="G24">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H24">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I24">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J24">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K24">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L24">
-        <v>23.68</v>
-      </c>
-      <c r="M24">
-        <v>18.62</v>
-      </c>
-      <c r="N24" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="M24" s="2">
         <v>1464</v>
       </c>
+      <c r="N24">
+        <v>0.9</v>
+      </c>
       <c r="O24">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P24">
         <v>4925.76</v>
@@ -2177,31 +2200,31 @@
         <v>0.8</v>
       </c>
       <c r="G25">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H25">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I25">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J25">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K25">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L25">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M25">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N25">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O25" s="2">
-        <v>22</v>
+        <v>0.8</v>
       </c>
       <c r="P25">
         <v>4925.76</v>
@@ -2227,31 +2250,31 @@
         <v>0.8</v>
       </c>
       <c r="G26">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H26">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I26">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J26">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K26">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L26">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M26">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N26">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O26" s="2">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="P26">
         <v>4925.76</v>
@@ -2277,31 +2300,31 @@
         <v>0.8</v>
       </c>
       <c r="G27">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H27">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I27">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J27">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K27">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L27">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M27">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N27">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O27">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P27" s="2">
         <v>2463</v>
@@ -2327,31 +2350,31 @@
         <v>0.8</v>
       </c>
       <c r="G28">
-        <v>0.32500000000000001</v>
+        <v>241.23</v>
       </c>
       <c r="H28">
-        <v>241.23</v>
+        <v>169.68</v>
       </c>
       <c r="I28">
-        <v>169.68</v>
+        <v>84.84</v>
       </c>
       <c r="J28">
-        <v>84.84</v>
+        <v>0.95</v>
       </c>
       <c r="K28">
-        <v>0.95</v>
+        <v>23.68</v>
       </c>
       <c r="L28">
-        <v>23.68</v>
+        <v>0.23</v>
       </c>
       <c r="M28">
-        <v>18.62</v>
+        <v>732</v>
       </c>
       <c r="N28">
-        <v>732</v>
+        <v>0.9</v>
       </c>
       <c r="O28">
-        <v>44.31</v>
+        <v>0.93</v>
       </c>
       <c r="P28" s="2">
         <v>9851</v>

</xml_diff>

<commit_message>
Sorted out tornado plots and nicer labels
</commit_message>
<xml_diff>
--- a/inst/extdata/scenario_input_values.xlsx
+++ b/inst/extdata/scenario_input_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\R\LTBIdiagTST\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E429BD9-78E2-4DD8-A4BF-A4C982131017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A3FB5-55E4-4151-AC6E-3DD0A0A6CDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,7 +954,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1809,7 @@
         <v>84.84</v>
       </c>
       <c r="J17" s="2">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="K17">
         <v>23.68</v>
@@ -2015,7 +2015,7 @@
         <v>23.68</v>
       </c>
       <c r="L21" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="M21">
         <v>732</v>
@@ -2065,7 +2065,7 @@
         <v>23.68</v>
       </c>
       <c r="L22" s="2">
-        <v>0.5</v>
+        <v>0.26</v>
       </c>
       <c r="M22">
         <v>732</v>

</xml_diff>